<commit_message>
finished hands and were evaluated
</commit_message>
<xml_diff>
--- a/doc/DadtaminingResults.xlsx
+++ b/doc/DadtaminingResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>C5.0</t>
   </si>
@@ -36,16 +36,31 @@
     <t>Configuration 1</t>
   </si>
   <si>
-    <t>Feature Selection (default)</t>
+    <t>Feature Sel (custom_1)</t>
   </si>
   <si>
-    <t>PAC Factor (default)</t>
+    <t>Feature Sel (default)</t>
   </si>
   <si>
-    <t>Feature Selection (custom)</t>
+    <t>PAC Fac (default)</t>
   </si>
   <si>
-    <t>PAC Factor (custom)</t>
+    <t>PAC Fac (custom_1)</t>
+  </si>
+  <si>
+    <t>Configuration 1 to 2</t>
+  </si>
+  <si>
+    <t>PAC Factor (compare_1_2)</t>
+  </si>
+  <si>
+    <t>PAC Fac (compare_2_2)</t>
+  </si>
+  <si>
+    <t>Feature Sel (compare_1_2)</t>
+  </si>
+  <si>
+    <t>Feature sel (compare_2_2)</t>
   </si>
 </sst>
 </file>
@@ -76,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -224,36 +239,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -348,30 +391,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$E$1</c:f>
+              <c:f>Tabelle1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Feature Selection (default)</c:v>
+                  <c:v>Feature Sel (default)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PAC Factor (default)</c:v>
+                  <c:v>PAC Fac (default)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Feature Selection (custom)</c:v>
+                  <c:v>Feature Sel (custom_1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>PAC Factor (custom)</c:v>
+                  <c:v>PAC Fac (custom_1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>PAC Factor (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PAC Fac (compare_2_2)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Feature Sel (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Feature sel (compare_2_2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$E$2</c:f>
+              <c:f>Tabelle1!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>410500</c:v>
                 </c:pt>
@@ -383,6 +438,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>437960</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>438350</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>416950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>396700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>370300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,30 +486,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$E$1</c:f>
+              <c:f>Tabelle1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Feature Selection (default)</c:v>
+                  <c:v>Feature Sel (default)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PAC Factor (default)</c:v>
+                  <c:v>PAC Fac (default)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Feature Selection (custom)</c:v>
+                  <c:v>Feature Sel (custom_1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>PAC Factor (custom)</c:v>
+                  <c:v>PAC Fac (custom_1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>PAC Factor (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PAC Fac (compare_2_2)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Feature Sel (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Feature sel (compare_2_2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$E$3</c:f>
+              <c:f>Tabelle1!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>409150</c:v>
                 </c:pt>
@@ -454,6 +533,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>426700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>438800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>427900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>437850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>425850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,30 +581,42 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$1:$E$1</c:f>
+              <c:f>Tabelle1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Feature Selection (default)</c:v>
+                  <c:v>Feature Sel (default)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PAC Factor (default)</c:v>
+                  <c:v>PAC Fac (default)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Feature Selection (custom)</c:v>
+                  <c:v>Feature Sel (custom_1)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>PAC Factor (custom)</c:v>
+                  <c:v>PAC Fac (custom_1)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>PAC Factor (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PAC Fac (compare_2_2)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Feature Sel (compare_1_2)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Feature sel (compare_2_2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$E$4</c:f>
+              <c:f>Tabelle1!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>393950</c:v>
                 </c:pt>
@@ -525,6 +628,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>419550</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>419550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>419550</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>393850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>393850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,15 +1394,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:colOff>1127758</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1612,102 +1727,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>410500</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="6">
         <v>428800</v>
       </c>
       <c r="D2" s="1">
         <v>396700</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="6">
         <v>437960</v>
       </c>
+      <c r="F2" s="17">
+        <v>438350</v>
+      </c>
+      <c r="G2" s="19">
+        <v>416950</v>
+      </c>
+      <c r="H2" s="18">
+        <v>396700</v>
+      </c>
+      <c r="I2" s="19">
+        <v>370300</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="7">
         <v>409150</v>
       </c>
       <c r="C3" s="2">
         <v>427450</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="7">
         <v>414800</v>
       </c>
       <c r="E3" s="2">
         <v>426700</v>
       </c>
+      <c r="F3" s="7">
+        <v>438800</v>
+      </c>
+      <c r="G3" s="2">
+        <v>427900</v>
+      </c>
+      <c r="H3" s="2">
+        <v>437850</v>
+      </c>
+      <c r="I3" s="2">
+        <v>425850</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>393950</v>
       </c>
       <c r="C4" s="3">
         <v>419450</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <v>394050</v>
       </c>
       <c r="E4" s="3">
         <v>419550</v>
       </c>
+      <c r="F4" s="8">
+        <v>419550</v>
+      </c>
+      <c r="G4" s="3">
+        <v>419550</v>
+      </c>
+      <c r="H4" s="20">
+        <v>393850</v>
+      </c>
+      <c r="I4" s="3">
+        <v>393850</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>